<commit_message>
All code done (needs cleaning)
</commit_message>
<xml_diff>
--- a/Morgagebond_rates.xlsx
+++ b/Morgagebond_rates.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophusschlosser/Documents/Whynot/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicklas/Whynot/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="150000" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;kr.&quot;;[Red]\-#,##0.00\ &quot;kr.&quot;"/>
   </numFmts>
@@ -86,6 +86,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -356,7 +359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -373,115 +378,115 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2019</v>
+        <v>1999</v>
       </c>
       <c r="B2">
-        <v>-0.44477</v>
+        <v>3.48</v>
       </c>
       <c r="C2">
-        <v>2.0364300000000002</v>
+        <v>6.19</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2018</v>
+        <v>2000</v>
       </c>
       <c r="B3">
-        <v>-0.59138000000000002</v>
+        <v>4.79</v>
       </c>
       <c r="C3">
-        <v>2.0469300000000001</v>
+        <v>7.25</v>
       </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>2017</v>
+        <v>2001</v>
       </c>
       <c r="B4">
-        <v>-0.44664999999999999</v>
+        <v>5.01</v>
       </c>
       <c r="C4">
-        <v>2.4649800000000002</v>
+        <v>6.74</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>2016</v>
+        <v>2002</v>
       </c>
       <c r="B5">
-        <v>1.2999999999999999E-2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="C5">
-        <v>2.7843599999999999</v>
+        <v>6.61</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2015</v>
+        <v>2003</v>
       </c>
       <c r="B6">
-        <v>-0.28000000000000003</v>
+        <v>2.62</v>
       </c>
       <c r="C6">
-        <v>2.16</v>
+        <v>5.5</v>
       </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>2014</v>
+        <v>2004</v>
       </c>
       <c r="B7">
-        <v>0.22763</v>
+        <v>2.17</v>
       </c>
       <c r="C7">
-        <v>3.3209399999999998</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>2013</v>
+        <v>2005</v>
       </c>
       <c r="B8">
-        <v>0.25979000000000002</v>
+        <v>2.37</v>
       </c>
       <c r="C8">
-        <v>3.3853800000000001</v>
+        <v>4.53</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>2012</v>
+        <v>2006</v>
       </c>
       <c r="B9">
-        <v>0.75</v>
+        <v>3.2</v>
       </c>
       <c r="C9">
-        <v>3.92</v>
+        <v>5.09</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="B10">
-        <v>1.72</v>
+        <v>4.24</v>
       </c>
       <c r="C10">
-        <v>5.03</v>
+        <v>5.18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="B11">
-        <v>1.3</v>
+        <v>4.3</v>
       </c>
       <c r="C11">
-        <v>4.79</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -497,115 +502,118 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B13">
-        <v>4.3</v>
+        <v>1.3</v>
       </c>
       <c r="C13">
-        <v>5.72</v>
+        <v>4.79</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>2007</v>
+        <v>2011</v>
       </c>
       <c r="B14">
-        <v>4.24</v>
+        <v>1.72</v>
       </c>
       <c r="C14">
-        <v>5.18</v>
+        <v>5.03</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="B15">
-        <v>3.2</v>
+        <v>0.75</v>
       </c>
       <c r="C15">
-        <v>5.09</v>
+        <v>3.92</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>2005</v>
+        <v>2013</v>
       </c>
       <c r="B16">
-        <v>2.37</v>
+        <v>0.25979000000000002</v>
       </c>
       <c r="C16">
-        <v>4.53</v>
+        <v>3.3853800000000001</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>2004</v>
+        <v>2014</v>
       </c>
       <c r="B17">
-        <v>2.17</v>
+        <v>0.22763</v>
       </c>
       <c r="C17">
-        <v>5.18</v>
+        <v>3.3209399999999998</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2003</v>
+        <v>2015</v>
       </c>
       <c r="B18">
-        <v>2.62</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="C18">
-        <v>5.5</v>
+        <v>2.16</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>2002</v>
+        <v>2016</v>
       </c>
       <c r="B19">
-        <v>4.0999999999999996</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="C19">
-        <v>6.61</v>
+        <v>2.7843599999999999</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>2001</v>
+        <v>2017</v>
       </c>
       <c r="B20">
-        <v>5.01</v>
+        <v>-0.44664999999999999</v>
       </c>
       <c r="C20">
-        <v>6.74</v>
+        <v>2.4649800000000002</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2000</v>
+        <v>2018</v>
       </c>
       <c r="B21">
-        <v>4.79</v>
+        <v>-0.59138000000000002</v>
       </c>
       <c r="C21">
-        <v>7.25</v>
+        <v>2.0469300000000001</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1999</v>
+        <v>2019</v>
       </c>
       <c r="B22">
-        <v>3.48</v>
+        <v>-0.44477</v>
       </c>
       <c r="C22">
-        <v>6.19</v>
+        <v>2.0364300000000002</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:C22">
+    <sortCondition ref="A2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>